<commit_message>
ExcelReader Convert To EditorWindow
</commit_message>
<xml_diff>
--- a/Assets/Scripts/1.Systems/Abilities/Effects/Resources/Documents/Ability/AbilityInfo.xlsx
+++ b/Assets/Scripts/1.Systems/Abilities/Effects/Resources/Documents/Ability/AbilityInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\myWorks\Unity-BolierPlate-Codes\Assets\Scripts\1.Abilities\Effects\Resources\Documents\Ability\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\myWorks\Unity-BolierPlate-Codes\Assets\Scripts\1.Systems\Abilities\Effects\Resources\Documents\Ability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52885671-2565-4704-9773-90E3D4D79EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDC908A-097C-4FF2-8138-39DCCEAE67C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14640" yWindow="3945" windowWidth="28800" windowHeight="15345" activeTab="5" xr2:uid="{4F09BE30-3FCF-46F0-A93C-3CEDA836A106}"/>
+    <workbookView xWindow="7605" yWindow="2730" windowWidth="28800" windowHeight="15345" xr2:uid="{4F09BE30-3FCF-46F0-A93C-3CEDA836A106}"/>
   </bookViews>
   <sheets>
     <sheet name="AreaAbility" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="20">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -99,6 +99,26 @@
   </si>
   <si>
     <t>MaxStackCount</t>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -467,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B2E12A-5366-4C7A-9667-41338698090D}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -509,7 +529,30 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H2" s="1"/>
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
@@ -595,11 +638,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H17:J17"/>
     <mergeCell ref="H12:J12"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="H2:J2"/>
@@ -612,6 +650,11 @@
     <mergeCell ref="H9:J9"/>
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H17:J17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -835,6 +878,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H5:J5"/>
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="H15:J15"/>
@@ -845,12 +894,6 @@
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="H11:J11"/>
     <mergeCell ref="H12:J12"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H5:J5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1087,8 +1130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62EF9C77-F5E5-4253-B080-E4A4AF2B33F0}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>